<commit_message>
Added the collaboration part
</commit_message>
<xml_diff>
--- a/given_data/fixedcosts.xlsx
+++ b/given_data/fixedcosts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuenl-my.sharepoint.com/personal/l_martin_tue_nl/Documents/Transportation Teaching/1CM110/2022/Block 2/Assignment/Shared Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4c0012dffc44a574/Documents/Masters/TUe/Q2/Descion Making/Assignment/Assignment 2/DecisionMaking_Assignment_3/given_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="11_AD4DB114E441178AC67DF4DEAE53CB7E683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E51C2AD2-9331-47C0-ACB7-5F06FD92BECC}"/>
+  <xr:revisionPtr revIDLastSave="64" documentId="11_AD4DB114E441178AC67DF4DEAE53CB7E683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1544E6FB-AF77-4692-B663-AB15BC727D6C}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1755" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fixed_cost" sheetId="1" r:id="rId1"/>
@@ -82,6 +82,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -111,11 +114,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -393,15 +397,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N14"/>
+  <dimension ref="A1:Q14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="P4" sqref="P4:Q9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -445,579 +449,613 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>12.5</v>
-      </c>
-      <c r="C2">
+      <c r="B2" s="1">
+        <v>12.5</v>
+      </c>
+      <c r="C2" s="1">
         <v>19.63008577301995</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>20.586027923844426</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>14.481282749439901</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="1">
         <v>24.125246156960959</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="1">
         <v>15.03713661132247</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="1">
         <v>19.830266518182388</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="1">
         <v>14.355268240455386</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="1">
         <v>25.692515671359217</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="1">
         <v>21.591933296470955</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="1">
         <v>17.502528559702611</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="1">
         <v>21.586991007514534</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="1">
         <v>20.657149137020514</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>19.63008577301995</v>
       </c>
-      <c r="C3">
-        <v>12.5</v>
-      </c>
-      <c r="D3">
+      <c r="C3" s="1">
+        <v>12.5</v>
+      </c>
+      <c r="D3" s="1">
         <v>15.86420295379256</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>20.681882072290719</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="1">
         <v>17.362218431873757</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="1">
         <v>20.637692807175586</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="1">
         <v>14.788181277265661</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="1">
         <v>18.289323938457287</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="1">
         <v>18.56446684742604</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="1">
         <v>18.611956717974937</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="1">
         <v>16.557731048950487</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="1">
         <v>17.503247772988324</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="1">
         <v>17.756442237342355</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>20.586027923844426</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>15.86420295379256</v>
       </c>
-      <c r="D4">
-        <v>12.5</v>
-      </c>
-      <c r="E4">
+      <c r="D4" s="1">
+        <v>12.5</v>
+      </c>
+      <c r="E4" s="1">
         <v>20.859080543744327</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="1">
         <v>16.650804629012406</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="1">
         <v>20.534213238575994</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="1">
         <v>18.152370599365515</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="1">
         <v>18.799565895181356</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="1">
         <v>19.340103715472036</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="1">
         <v>15.310982968912169</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="1">
         <v>19.40823142454645</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="1">
         <v>14.142714846067813</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="1">
         <v>21.111872824262896</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>14.481282749439901</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>20.681882072290719</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>20.859080543744327</v>
       </c>
-      <c r="E5">
-        <v>12.5</v>
-      </c>
-      <c r="F5">
+      <c r="E5" s="1">
+        <v>12.5</v>
+      </c>
+      <c r="F5" s="1">
         <v>24.751585764964233</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="1">
         <v>13.207884367462533</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="1">
         <v>21.315763396987329</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="1">
         <v>14.896655141505688</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="1">
         <v>26.686781502994741</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="1">
         <v>21.23479898371933</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="1">
         <v>19.280236911726735</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="1">
         <v>21.537230993405277</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="1">
         <v>22.488488269940646</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>24.125246156960959</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>17.362218431873757</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>16.650804629012406</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <v>24.751585764964233</v>
       </c>
-      <c r="F6">
-        <v>12.5</v>
-      </c>
-      <c r="G6">
+      <c r="F6" s="1">
+        <v>12.5</v>
+      </c>
+      <c r="G6" s="1">
         <v>24.512240049179024</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="1">
         <v>18.904650345842555</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="1">
         <v>22.501102674570529</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="1">
         <v>15.639651761593775</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="1">
         <v>18.464744744370172</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="1">
         <v>21.353050270283951</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="1">
         <v>17.10668524092878</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="1">
         <v>21.600702931795389</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>15.03713661132247</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>20.637692807175586</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>20.534213238575994</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="1">
         <v>13.207884367462533</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="1">
         <v>24.512240049179024</v>
       </c>
-      <c r="G7">
-        <v>12.5</v>
-      </c>
-      <c r="H7">
+      <c r="G7" s="1">
+        <v>12.5</v>
+      </c>
+      <c r="H7" s="1">
         <v>21.451646952717347</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="1">
         <v>14.960354403835503</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="1">
         <v>26.574177233946585</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="1">
         <v>20.720130038725479</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="1">
         <v>19.592982829447251</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="1">
         <v>21.105612750079096</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="1">
         <v>22.814463388974989</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>19.830266518182388</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>14.788181277265661</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <v>18.152370599365515</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="1">
         <v>21.315763396987329</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="1">
         <v>18.904650345842555</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="1">
         <v>21.451646952717347</v>
       </c>
-      <c r="H8">
-        <v>12.5</v>
-      </c>
-      <c r="I8">
+      <c r="H8" s="1">
+        <v>12.5</v>
+      </c>
+      <c r="I8" s="1">
         <v>18.991305032176015</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="1">
         <v>19.059549157186609</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="1">
         <v>20.884906469597595</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="1">
         <v>15.342818520170429</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="1">
         <v>19.791039482875526</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="1">
         <v>15.483905393088271</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>14.355268240455386</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>18.289323938457287</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <v>18.799565895181356</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="1">
         <v>14.896655141505688</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="1">
         <v>22.501102674570529</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="1">
         <v>14.960354403835503</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="1">
         <v>18.991305032176015</v>
       </c>
-      <c r="I9">
-        <v>12.5</v>
-      </c>
-      <c r="J9">
+      <c r="I9" s="1">
+        <v>12.5</v>
+      </c>
+      <c r="J9" s="1">
         <v>24.313659061007151</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="1">
         <v>19.741897634306543</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="1">
         <v>17.265266950307002</v>
       </c>
-      <c r="M9">
+      <c r="M9" s="1">
         <v>19.740780630678138</v>
       </c>
-      <c r="N9">
+      <c r="N9" s="1">
         <v>20.474098214250809</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>25.692515671359217</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <v>18.56446684742604</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <v>19.340103715472036</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="1">
         <v>26.686781502994741</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="1">
         <v>15.639651761593775</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="1">
         <v>26.574177233946585</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="1">
         <v>19.059549157186609</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="1">
         <v>24.313659061007151</v>
       </c>
-      <c r="J10">
-        <v>12.5</v>
-      </c>
-      <c r="K10">
+      <c r="J10" s="1">
+        <v>12.5</v>
+      </c>
+      <c r="K10" s="1">
         <v>21.524582270633452</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="1">
         <v>21.880589425073538</v>
       </c>
-      <c r="M10">
+      <c r="M10" s="1">
         <v>20.131676213224623</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="1">
         <v>21.004657135073202</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>21.591933296470955</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>18.611956717974937</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <v>15.310982968912169</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="1">
         <v>21.23479898371933</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="1">
         <v>18.464744744370172</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="1">
         <v>20.720130038725479</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="1">
         <v>20.884906469597595</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="1">
         <v>19.741897634306543</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="1">
         <v>21.524582270633452</v>
       </c>
-      <c r="K11">
-        <v>12.5</v>
-      </c>
-      <c r="L11">
+      <c r="K11" s="1">
+        <v>12.5</v>
+      </c>
+      <c r="L11" s="1">
         <v>21.736819088696791</v>
       </c>
-      <c r="M11">
+      <c r="M11" s="1">
         <v>13.909631442173538</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="1">
         <v>23.798000177446717</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <v>17.502528559702611</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <v>16.557731048950487</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="1">
         <v>19.40823142454645</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="1">
         <v>19.280236911726735</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="1">
         <v>21.353050270283951</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="1">
         <v>19.592982829447251</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="1">
         <v>15.342818520170429</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="1">
         <v>17.265266950307002</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="1">
         <v>21.880589425073538</v>
       </c>
-      <c r="K12">
+      <c r="K12" s="1">
         <v>21.736819088696791</v>
       </c>
-      <c r="L12">
-        <v>12.5</v>
-      </c>
-      <c r="M12">
+      <c r="L12" s="1">
+        <v>12.5</v>
+      </c>
+      <c r="M12" s="1">
         <v>20.978478724727239</v>
       </c>
-      <c r="N12">
+      <c r="N12" s="1">
         <v>15.721940466172503</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <v>21.586991007514534</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <v>17.503247772988324</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="1">
         <v>14.142714846067813</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="1">
         <v>21.537230993405277</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="1">
         <v>17.10668524092878</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="1">
         <v>21.105612750079096</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="1">
         <v>19.791039482875526</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="1">
         <v>19.740780630678138</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="1">
         <v>20.131676213224623</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="1">
         <v>13.909631442173538</v>
       </c>
-      <c r="L13">
+      <c r="L13" s="1">
         <v>20.978478724727239</v>
       </c>
-      <c r="M13">
-        <v>12.5</v>
-      </c>
-      <c r="N13">
+      <c r="M13" s="1">
+        <v>12.5</v>
+      </c>
+      <c r="N13" s="1">
         <v>22.754151309703314</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
         <v>20.657149137020514</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="1">
         <v>17.756442237342355</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="1">
         <v>21.111872824262896</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="1">
         <v>22.488488269940646</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="1">
         <v>21.600702931795389</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="1">
         <v>22.814463388974989</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="1">
         <v>15.483905393088271</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="1">
         <v>20.474098214250809</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="1">
         <v>21.004657135073202</v>
       </c>
-      <c r="K14">
+      <c r="K14" s="1">
         <v>23.798000177446717</v>
       </c>
-      <c r="L14">
+      <c r="L14" s="1">
         <v>15.721940466172503</v>
       </c>
-      <c r="M14">
+      <c r="M14" s="1">
         <v>22.754151309703314</v>
       </c>
-      <c r="N14">
+      <c r="N14" s="1">
         <v>12.5</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:N14">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P5:Q9">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>